<commit_message>
Adapted evaluation code for final experiment run
</commit_message>
<xml_diff>
--- a/Past_experiments/Final_experiment/collected_data/data.xlsx
+++ b/Past_experiments/Final_experiment/collected_data/data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="83">
   <si>
     <t xml:space="preserve">participant</t>
   </si>
@@ -58,25 +58,217 @@
     <t xml:space="preserve">TIME_total</t>
   </si>
   <si>
-    <t xml:space="preserve">s.608b3790-a526-4925-9ef1-b8f529dd9713.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rosch7_Final.2022-11-23-1323.data.608b3790-a526-4925-9ef1-b8f529dd9713.txt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">628d0f57a17caac1888983d2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">637dfad72423f07435969c0c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0feu6b8mpt9p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-11-23-12-58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-11-23-13-23</t>
+    <t xml:space="preserve">s.6dfe81c1-4290-4cb0-b762-2b62276396b4.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1008.data.6dfe81c1-4290-4cb0-b762-2b62276396b4.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60e55bb59cfd0aa9803b4470</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2ac7f6c1f58ea63eeae1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2f0872424308332f4fee</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.120b6e6b-37e0-4021-9ccb-28c9795ec4eb.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1027.data.120b6e6b-37e0-4021-9ccb-28c9795ec4eb.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6299dc2997f47665304008b7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2ec3b7fb7dcb422b2a09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.1511d81c-e04b-4fed-8967-8058e8f35f78.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1008.data.1511d81c-e04b-4fed-8967-8058e8f35f78.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Didn't know some names were a term for some objects.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59ba7072b06d2b0001583e33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2ac7f6c1f58ea63eeae2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2e606804f95551030be9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.de1592ad-0f5b-4dde-923a-e8703e87d474.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1010.data.de1592ad-0f5b-4dde-923a-e8703e87d474.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">614a144baf10bcf4807d2652</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2d8a5bcf1e7bf6030bba</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.6170529f-29bd-4b97-b800-d14eb78a7f9c.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1012.data.6170529f-29bd-4b97-b800-d14eb78a7f9c.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">577d9254c6144900014a0083</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2ddd67372e1bef2f4ffe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.054de82a-7835-4f1b-83b3-af17e39d7d41.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1014.data.054de82a-7835-4f1b-83b3-af17e39d7d41.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55f2786632af7400051704aa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2e9e62fbfac49e969bfb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.e3b607e0-6916-4ba8-bd19-ab668922f3b8.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1038.data.e3b607e0-6916-4ba8-bd19-ab668922f3b8.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ec509f11a1793424f0b8ee4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2e56f8b7a7822bd9e175</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.cf54b2bc-0a1e-4ba2-b365-ffca72e64215.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1000.data.cf54b2bc-0a1e-4ba2-b365-ffca72e64215.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">610427f727bda2e1bb54085e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2d7d27622c6b292b2a42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.cf80aa70-b278-413a-b6aa-9809ca09433d.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1008.data.cf80aa70-b278-413a-b6aa-9809ca09433d.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5c28d36b6fbaed00010847a8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2f60551954419de37a9a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.48c5ec77-ccdd-42d7-9ca4-95199ba994fc.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1017.data.48c5ec77-ccdd-42d7-9ca4-95199ba994fc.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5ba3be96258e340001cebb06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2fa1a166a3765d9b9c45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.e7d2b7c7-696e-44a8-8d7a-052fd9297eb6.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1014.data.e7d2b7c7-696e-44a8-8d7a-052fd9297eb6.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57bafa6cc308ca00014527c2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2ce8f07e2a82f0b377f9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s.e0aa6604-dd5f-4a5a-9316-20c0e04630b8.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosch7_Final.2022-11-24-1022.data.e0aa6604-dd5f-4a5a-9316-20c0e04630b8.txt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60d6e4277e58667c5ce46f7f</t>
+  </si>
+  <si>
+    <t xml:space="preserve">637f2fbf64879cee5493059a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-09-49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-11-24-10-23</t>
   </si>
 </sst>
 </file>
@@ -172,7 +364,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -180,15 +372,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="66.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="66.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="46.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="24.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="24.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="23.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="0" width="15.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.46"/>
   </cols>
@@ -236,16 +428,16 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="0" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="0" t="s">
         <v>14</v>
@@ -263,7 +455,395 @@
         <v>18</v>
       </c>
       <c r="L2" s="0" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>25</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="L13" s="0" t="n">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>